<commit_message>
Fix typo in Excel file
</commit_message>
<xml_diff>
--- a/Microsoft.xlsx
+++ b/Microsoft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/em/Downloads/pythonpractice/NEAD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AFF30B-4C75-2248-9D91-5AD26A4ADC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6609041-1708-CF45-85D7-07A7B44D91F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Microsoft" sheetId="1" r:id="rId1"/>
@@ -77,6 +77,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -516,7 +520,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -559,11 +563,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -591,6 +598,7 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="42" builtinId="3"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -920,7 +928,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -943,7 +951,7 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>5982</v>
       </c>
     </row>
@@ -954,7 +962,7 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>4689</v>
       </c>
     </row>
@@ -965,7 +973,7 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>4643</v>
       </c>
     </row>
@@ -976,7 +984,7 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>1885</v>
       </c>
     </row>
@@ -987,7 +995,7 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>1429</v>
       </c>
     </row>
@@ -998,7 +1006,7 @@
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>1355</v>
       </c>
     </row>
@@ -1009,7 +1017,7 @@
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>1362</v>
       </c>
     </row>
@@ -1020,7 +1028,7 @@
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1031,7 +1039,7 @@
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>583</v>
       </c>
     </row>
@@ -1042,7 +1050,7 @@
       <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>21928</v>
       </c>
     </row>
@@ -1053,7 +1061,7 @@
       <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>6439</v>
       </c>
     </row>
@@ -1064,7 +1072,7 @@
       <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>5332</v>
       </c>
     </row>
@@ -1075,7 +1083,7 @@
       <c r="B14" t="s">
         <v>6</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>4805</v>
       </c>
     </row>
@@ -1086,7 +1094,7 @@
       <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>3617</v>
       </c>
     </row>
@@ -1097,7 +1105,7 @@
       <c r="B16" t="s">
         <v>8</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>1605</v>
       </c>
     </row>
@@ -1108,7 +1116,7 @@
       <c r="B17" t="s">
         <v>9</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>1371</v>
       </c>
     </row>
@@ -1119,7 +1127,7 @@
       <c r="B18" t="s">
         <v>10</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>1697</v>
       </c>
     </row>
@@ -1130,7 +1138,7 @@
       <c r="B19" t="s">
         <v>11</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>228</v>
       </c>
     </row>
@@ -1141,7 +1149,7 @@
       <c r="B20" t="s">
         <v>12</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>732</v>
       </c>
     </row>
@@ -1152,7 +1160,7 @@
       <c r="B21" t="s">
         <v>16</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>25826</v>
       </c>
     </row>
@@ -1163,7 +1171,7 @@
       <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>6234</v>
       </c>
     </row>
@@ -1174,7 +1182,7 @@
       <c r="B23" t="s">
         <v>5</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>5297</v>
       </c>
     </row>
@@ -1185,7 +1193,7 @@
       <c r="B24" t="s">
         <v>6</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>4253</v>
       </c>
     </row>
@@ -1196,7 +1204,7 @@
       <c r="B25" t="s">
         <v>7</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>1906</v>
       </c>
     </row>
@@ -1207,7 +1215,7 @@
       <c r="B26" t="s">
         <v>8</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>1599</v>
       </c>
     </row>
@@ -1218,7 +1226,7 @@
       <c r="B27" t="s">
         <v>9</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>1383</v>
       </c>
     </row>
@@ -1229,7 +1237,7 @@
       <c r="B28" t="s">
         <v>10</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>958</v>
       </c>
     </row>
@@ -1240,7 +1248,7 @@
       <c r="B29" t="s">
         <v>11</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>976</v>
       </c>
     </row>
@@ -1251,7 +1259,7 @@
       <c r="B30" t="s">
         <v>12</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>606</v>
       </c>
     </row>
@@ -1262,7 +1270,7 @@
       <c r="B31" t="s">
         <v>16</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>23212</v>
       </c>
     </row>
@@ -1273,7 +1281,7 @@
       <c r="B32" t="s">
         <v>4</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>25573</v>
       </c>
     </row>
@@ -1284,7 +1292,7 @@
       <c r="B33" t="s">
         <v>5</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>21649</v>
       </c>
     </row>
@@ -1295,7 +1303,7 @@
       <c r="B34" t="s">
         <v>6</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>18593</v>
       </c>
     </row>
@@ -1306,7 +1314,7 @@
       <c r="B35" t="s">
         <v>7</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>9051</v>
       </c>
     </row>
@@ -1317,7 +1325,7 @@
       <c r="B36" t="s">
         <v>8</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <v>6219</v>
       </c>
     </row>
@@ -1328,7 +1336,7 @@
       <c r="B37" t="s">
         <v>9</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>5542</v>
       </c>
     </row>
@@ -1339,7 +1347,7 @@
       <c r="B38" t="s">
         <v>10</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>5062</v>
       </c>
     </row>
@@ -1350,7 +1358,7 @@
       <c r="B39" t="s">
         <v>11</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <v>2271</v>
       </c>
     </row>
@@ -1361,7 +1369,7 @@
       <c r="B40" t="s">
         <v>12</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <v>2611</v>
       </c>
     </row>
@@ -1372,7 +1380,7 @@
       <c r="B41" t="s">
         <v>16</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <v>96571</v>
       </c>
     </row>

</xml_diff>